<commit_message>
Fixed Omega computer obj and removed achievement
</commit_message>
<xml_diff>
--- a/Achievement Tracker.xlsx
+++ b/Achievement Tracker.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan Leich\Documents\GitHub\Improved Unlockables\Improved-Unlockables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cprin\Documents\GitHub\Improved-Unlockables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8507E3-98E4-42E5-B090-C2F23CFF07BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAF98F9-BDF2-42BE-BD15-C48A6B6454AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$B$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$B$53</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Achievement Name</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>A Spy Game (Custom Achievement)</t>
-  </si>
-  <si>
-    <t>The Legacy Virus (Custom Achievement)</t>
   </si>
   <si>
     <t>Mutual Respect (Custom Achievement)</t>
@@ -348,9 +345,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
@@ -359,29 +353,7 @@
       </extLst>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9E1F2"/>
-          <bgColor rgb="FFD9E1F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -419,7 +391,29 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -427,6 +421,9 @@
           <color rgb="FF8EA9DB"/>
         </left>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -482,11 +479,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73806510-1F6C-4AC8-8B2C-27038AAB5244}" name="Table1" displayName="Table1" ref="A1:B55" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="4" tableBorderDxfId="5">
-  <autoFilter ref="A1:B54" xr:uid="{FF66C5D9-ED34-8F49-9B1C-C38D8DEA47EB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73806510-1F6C-4AC8-8B2C-27038AAB5244}" name="Table1" displayName="Table1" ref="A1:B54" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:B53" xr:uid="{FF66C5D9-ED34-8F49-9B1C-C38D8DEA47EB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C321B8E8-0265-46CB-984A-86660BB68D40}" name="Achievement Name" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4A463D9A-9910-4C6B-83BA-16664CDACDE1}" name="Unlocked" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C321B8E8-0265-46CB-984A-86660BB68D40}" name="Achievement Name" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4A463D9A-9910-4C6B-83BA-16664CDACDE1}" name="Unlocked" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -792,9 +789,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -809,10 +808,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <f>COUNTIF(B2:B54, TRUE) / COUNTA(A2:A54) * 100</f>
+        <f>COUNTIF(B2:B53, TRUE) / COUNTA(A2:A53) * 100</f>
         <v>0</v>
       </c>
     </row>
@@ -1156,7 +1155,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="9" t="b">
@@ -1164,7 +1163,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="9" t="b">
@@ -1172,7 +1171,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="9" t="b">
@@ -1180,15 +1179,15 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="9" t="b">
@@ -1196,15 +1195,15 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="9" t="b">
@@ -1212,15 +1211,15 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="9" t="b">
@@ -1228,7 +1227,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="9" t="b">
@@ -1236,20 +1235,12 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" s="1">
+      <c r="A54" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="1">
         <f>SUBTOTAL(103,Table1[Unlocked])</f>
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>